<commit_message>
Vanilla Expanded Framework 업데이트
</commit_message>
<xml_diff>
--- a/Data/Vanilla Expanded/Vanilla Expanded Framework - 2023507013/2023507013.xlsx
+++ b/Data/Vanilla Expanded/Vanilla Expanded Framework - 2023507013/2023507013.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\RimWorld\Mods\RMK\Data\Vanilla Expanded\Vanilla Expanded Framework - 2023507013\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6448CF-0C35-4A74-BF31-F6B86412ECE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A144776B-7202-4D38-A193-B2EB61FE6F46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1147,6 +1147,94 @@
         </r>
       </text>
     </comment>
+    <comment ref="E540" authorId="0" shapeId="0" xr:uid="{BF9D67FF-EEDB-43C1-B16E-449AD7B8A31F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Desc</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>에는</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>메서드</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>적용</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>필요</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="E567" authorId="0" shapeId="0" xr:uid="{7534E7C2-21F2-4328-96C6-E976AE943627}">
       <text>
         <r>
@@ -5636,7 +5724,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9272" uniqueCount="2432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9279" uniqueCount="2456">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -13154,12 +13242,108 @@
     <t>VWE - Laser</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>Gizmo Label</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gizmo Desc</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>계획 초기화</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>진행 중인 과정이 완료되면 새로운 작업을 시작하지 않고 설정을 초기화한 채 대기 상태로 둡니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>\n필요 온도: {0} - {1}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IP_LightDestroysWarning</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{0}(이)가 가공을 시작하려면 밝기가 적절한 범위에 있어야 합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{0}(이)가 가공을 시작하려면 온도가 적절한 범위({1} - {2})에 있어야 합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{0}(이)가 가공을 시작하려면 전원이 필요합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{0}(이)가 가공을 시작하려면 연료가 필요합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>VBE 위스키통</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>적절하지 않은 밝기로 인해 내용물이 손상되었습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>적절하지 않은 온도로 인해 내용물이 손상되었습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>적절하지 않은 밝기로 인해 가공이 중단되었습니다. 곧바로 해결하지 않으면 내용물이 손상됩니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>적절하지 않은 온도로 인해 가공이 중단되었습니다. 곧바로 해결하지 않으면 내용물이 손상됩니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{0}(이)가 가공을 시작하려면 비를 맞혀선 안됩니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>비를 맞아서 가공이 중단되었습니다. 곧바로 해결하지 않는다면 내용물이 손상됩니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>비를 맞아서 내용물이 손상되었습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>동작 확인</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>일반 설정</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>토글 패치</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>변경된 설정을 적용하려면 게임을 다시 시작해야 합니다</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>기존 세이브에 신규 세력 추가</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>기존 세이브 파일을 불러온 뒤 설정을 다시 확인해주세요</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -13237,8 +13421,17 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -13290,8 +13483,13 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -13405,8 +13603,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
@@ -13423,8 +13636,11 @@
     <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -13450,8 +13666,10 @@
     <xf numFmtId="49" fontId="4" fillId="7" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="9" xfId="6" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
+    <cellStyle name="계산" xfId="6" builtinId="22"/>
     <cellStyle name="나쁨" xfId="5" builtinId="27"/>
     <cellStyle name="메모" xfId="4" builtinId="10"/>
     <cellStyle name="보통" xfId="3" builtinId="28"/>
@@ -13759,8 +13977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C8A8E60-C272-4034-9D57-33A4FC3F4784}">
   <dimension ref="A1:F632"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A258" workbookViewId="0">
+      <selection activeCell="F275" sqref="F275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -18045,7 +18263,7 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="257" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A257" s="1" t="s">
         <v>694</v>
       </c>
@@ -18062,7 +18280,7 @@
         <v>1901</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="258" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A258" s="1" t="s">
         <v>697</v>
       </c>
@@ -18079,7 +18297,7 @@
         <v>1899</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="259" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A259" s="1" t="s">
         <v>700</v>
       </c>
@@ -18096,7 +18314,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="260" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A260" s="1" t="s">
         <v>703</v>
       </c>
@@ -18109,11 +18327,11 @@
       <c r="D260" s="1" t="s">
         <v>705</v>
       </c>
-      <c r="E260" s="7" t="s">
-        <v>2326</v>
-      </c>
-    </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E260" s="6" t="s">
+        <v>2440</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A261" s="1" t="s">
         <v>706</v>
       </c>
@@ -18126,11 +18344,11 @@
       <c r="D261" s="1" t="s">
         <v>708</v>
       </c>
-      <c r="E261" s="7" t="s">
-        <v>2327</v>
-      </c>
-    </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E261" s="6" t="s">
+        <v>2441</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A262" s="1" t="s">
         <v>709</v>
       </c>
@@ -18138,16 +18356,19 @@
         <v>505</v>
       </c>
       <c r="C262" s="1" t="s">
-        <v>710</v>
+        <v>2437</v>
       </c>
       <c r="D262" s="1" t="s">
         <v>711</v>
       </c>
-      <c r="E262" s="1" t="s">
-        <v>1911</v>
-      </c>
-    </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E262" s="6" t="s">
+        <v>2438</v>
+      </c>
+      <c r="F262" s="8" t="s">
+        <v>2442</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A263" s="1" t="s">
         <v>712</v>
       </c>
@@ -18160,11 +18381,11 @@
       <c r="D263" s="1" t="s">
         <v>714</v>
       </c>
-      <c r="E263" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E263" s="6" t="s">
+        <v>2447</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A264" s="1" t="s">
         <v>715</v>
       </c>
@@ -18177,11 +18398,11 @@
       <c r="D264" s="10" t="s">
         <v>717</v>
       </c>
-      <c r="E264" s="10" t="s">
-        <v>1930</v>
-      </c>
-    </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E264" s="13" t="s">
+        <v>2439</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A265" s="1" t="s">
         <v>718</v>
       </c>
@@ -18194,11 +18415,14 @@
       <c r="D265" s="1" t="s">
         <v>720</v>
       </c>
-      <c r="E265" s="6" t="s">
+      <c r="E265" s="7" t="s">
         <v>2232</v>
       </c>
-    </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F265" s="25" t="s">
+        <v>2450</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A266" s="1" t="s">
         <v>721</v>
       </c>
@@ -18211,11 +18435,11 @@
       <c r="D266" s="10" t="s">
         <v>723</v>
       </c>
-      <c r="E266" s="13" t="s">
+      <c r="E266" s="15" t="s">
         <v>2232</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="267" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A267" s="1" t="s">
         <v>724</v>
       </c>
@@ -18232,7 +18456,7 @@
         <v>2233</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="268" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A268" s="1" t="s">
         <v>727</v>
       </c>
@@ -18249,7 +18473,7 @@
         <v>1909</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="269" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A269" s="1" t="s">
         <v>730</v>
       </c>
@@ -18266,7 +18490,7 @@
         <v>2324</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="270" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A270" s="1" t="s">
         <v>732</v>
       </c>
@@ -18283,7 +18507,7 @@
         <v>2324</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="271" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A271" s="1" t="s">
         <v>735</v>
       </c>
@@ -18300,7 +18524,7 @@
         <v>2324</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="272" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A272" s="1" t="s">
         <v>738</v>
       </c>
@@ -18449,8 +18673,11 @@
       <c r="D280" s="1" t="s">
         <v>763</v>
       </c>
-      <c r="E280" s="1" t="s">
-        <v>1924</v>
+      <c r="E280" s="6" t="s">
+        <v>2434</v>
+      </c>
+      <c r="F280" s="8" t="s">
+        <v>2432</v>
       </c>
     </row>
     <row r="281" spans="1:6" x14ac:dyDescent="0.45">
@@ -18466,8 +18693,11 @@
       <c r="D281" s="1" t="s">
         <v>766</v>
       </c>
-      <c r="E281" s="1" t="s">
-        <v>1925</v>
+      <c r="E281" s="6" t="s">
+        <v>2435</v>
+      </c>
+      <c r="F281" s="8" t="s">
+        <v>2433</v>
       </c>
     </row>
     <row r="282" spans="1:6" x14ac:dyDescent="0.45">
@@ -18653,19 +18883,19 @@
       </c>
     </row>
     <row r="292" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A292" s="1" t="s">
+      <c r="A292" s="10" t="s">
         <v>797</v>
       </c>
-      <c r="B292" s="1" t="s">
-        <v>505</v>
-      </c>
-      <c r="C292" s="1" t="s">
+      <c r="B292" s="10" t="s">
+        <v>505</v>
+      </c>
+      <c r="C292" s="10" t="s">
         <v>798</v>
       </c>
-      <c r="D292" s="1" t="s">
+      <c r="D292" s="10" t="s">
         <v>799</v>
       </c>
-      <c r="E292" s="1" t="s">
+      <c r="E292" s="10" t="s">
         <v>1917</v>
       </c>
     </row>
@@ -18682,8 +18912,11 @@
       <c r="D293" s="1" t="s">
         <v>802</v>
       </c>
-      <c r="E293" s="1" t="s">
-        <v>1916</v>
+      <c r="E293" s="6" t="s">
+        <v>2445</v>
+      </c>
+      <c r="F293" s="8" t="s">
+        <v>2442</v>
       </c>
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.45">
@@ -18699,8 +18932,8 @@
       <c r="D294" s="1" t="s">
         <v>805</v>
       </c>
-      <c r="E294" s="1" t="s">
-        <v>1927</v>
+      <c r="E294" s="6" t="s">
+        <v>2443</v>
       </c>
     </row>
     <row r="295" spans="1:6" x14ac:dyDescent="0.45">
@@ -18716,8 +18949,8 @@
       <c r="D295" s="1" t="s">
         <v>808</v>
       </c>
-      <c r="E295" s="1" t="s">
-        <v>1910</v>
+      <c r="E295" s="6" t="s">
+        <v>2448</v>
       </c>
     </row>
     <row r="296" spans="1:6" x14ac:dyDescent="0.45">
@@ -18733,8 +18966,8 @@
       <c r="D296" s="1" t="s">
         <v>811</v>
       </c>
-      <c r="E296" s="1" t="s">
-        <v>1928</v>
+      <c r="E296" s="6" t="s">
+        <v>2449</v>
       </c>
     </row>
     <row r="297" spans="1:6" x14ac:dyDescent="0.45">
@@ -18750,25 +18983,25 @@
       <c r="D297" s="1" t="s">
         <v>814</v>
       </c>
-      <c r="E297" s="1" t="s">
-        <v>1934</v>
+      <c r="E297" s="6" t="s">
+        <v>2446</v>
       </c>
     </row>
     <row r="298" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A298" s="1" t="s">
+      <c r="A298" s="10" t="s">
         <v>815</v>
       </c>
-      <c r="B298" s="1" t="s">
-        <v>505</v>
-      </c>
-      <c r="C298" s="1" t="s">
+      <c r="B298" s="10" t="s">
+        <v>505</v>
+      </c>
+      <c r="C298" s="10" t="s">
         <v>816</v>
       </c>
-      <c r="D298" s="1" t="s">
+      <c r="D298" s="10" t="s">
         <v>817</v>
       </c>
-      <c r="E298" s="1" t="s">
-        <v>1929</v>
+      <c r="E298" s="13" t="s">
+        <v>2444</v>
       </c>
     </row>
     <row r="299" spans="1:6" x14ac:dyDescent="0.45">
@@ -18785,7 +19018,7 @@
         <v>820</v>
       </c>
       <c r="E299" s="6" t="s">
-        <v>2241</v>
+        <v>2436</v>
       </c>
     </row>
     <row r="300" spans="1:6" x14ac:dyDescent="0.45">
@@ -22547,24 +22780,24 @@
         <v>2103</v>
       </c>
     </row>
-    <row r="520" spans="1:5" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A520" s="1" t="s">
+    <row r="520" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A520" s="10" t="s">
         <v>1477</v>
       </c>
-      <c r="B520" s="1" t="s">
-        <v>505</v>
-      </c>
-      <c r="C520" s="1" t="s">
+      <c r="B520" s="10" t="s">
+        <v>505</v>
+      </c>
+      <c r="C520" s="10" t="s">
         <v>1478</v>
       </c>
-      <c r="D520" s="1" t="s">
+      <c r="D520" s="10" t="s">
         <v>1479</v>
       </c>
-      <c r="E520" s="1" t="s">
+      <c r="E520" s="10" t="s">
         <v>2105</v>
       </c>
     </row>
-    <row r="521" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="521" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A521" s="1" t="s">
         <v>1480</v>
       </c>
@@ -22577,9 +22810,11 @@
       <c r="D521" s="1" t="s">
         <v>1482</v>
       </c>
-      <c r="E521" s="5"/>
-    </row>
-    <row r="522" spans="1:5" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="E521" s="7" t="s">
+        <v>2451</v>
+      </c>
+    </row>
+    <row r="522" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A522" s="1" t="s">
         <v>1483</v>
       </c>
@@ -22626,7 +22861,9 @@
       <c r="D524" s="1" t="s">
         <v>1491</v>
       </c>
-      <c r="E524" s="1"/>
+      <c r="E524" s="7" t="s">
+        <v>2452</v>
+      </c>
     </row>
     <row r="525" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A525" s="1" t="s">
@@ -22641,8 +22878,8 @@
       <c r="D525" s="1" t="s">
         <v>1494</v>
       </c>
-      <c r="E525" s="1" t="s">
-        <v>2113</v>
+      <c r="E525" s="7" t="s">
+        <v>2453</v>
       </c>
     </row>
     <row r="526" spans="1:5" x14ac:dyDescent="0.45">
@@ -22709,8 +22946,8 @@
       <c r="D529" s="1" t="s">
         <v>1506</v>
       </c>
-      <c r="E529" s="1" t="s">
-        <v>2112</v>
+      <c r="E529" s="7" t="s">
+        <v>2454</v>
       </c>
     </row>
     <row r="530" spans="1:5" x14ac:dyDescent="0.45">
@@ -22726,8 +22963,8 @@
       <c r="D530" s="1" t="s">
         <v>1509</v>
       </c>
-      <c r="E530" s="1" t="s">
-        <v>2114</v>
+      <c r="E530" s="7" t="s">
+        <v>2455</v>
       </c>
     </row>
     <row r="531" spans="1:5" x14ac:dyDescent="0.45">

</xml_diff>